<commit_message>
updated vars and data
</commit_message>
<xml_diff>
--- a/ref/data_tables_and_derivations/ENERGY/eia_outlooks_table_8.2.xlsx
+++ b/ref/data_tables_and_derivations/ENERGY/eia_outlooks_table_8.2.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/lac_decarbonization/ref/ipcc_data_tables_and_derivations/ENERGY/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/lac_decarbonization/ref/data_tables_and_derivations/ENERGY/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0FE12E5-68C0-124C-A98B-BD28E911E41A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C42A383-18FD-A046-A661-F3AD45D6D771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="460" windowWidth="17220" windowHeight="14900" xr2:uid="{1C2313C9-7074-F343-BBF1-1D2E42E9CC1F}"/>
+    <workbookView xWindow="1300" yWindow="500" windowWidth="27620" windowHeight="18780" xr2:uid="{1C2313C9-7074-F343-BBF1-1D2E42E9CC1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,6 +28,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -503,10 +504,13 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="28.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>